<commit_message>
Updated documentation. Added links to the pristine resources
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/OECD-SIGI/SIGI_Recap.xlsx
+++ b/Simple_XLS_Importer/data/OECD-SIGI/SIGI_Recap.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="960" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="2355" yWindow="960" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SIGI_recap" sheetId="1" r:id="rId1"/>
+    <sheet name="links" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
   <si>
     <t>SIGI _ Recap</t>
   </si>
@@ -112,13 +113,88 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>Gender, Institutions and Development (Edition 2014)</t>
+  </si>
+  <si>
+    <t>http://www.oecd-ilibrary.org/development/data/oecd-international-development-statistics/gender-institutions-and-development-2014_data-00728-en</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/viewhtml.aspx?datasetcode=GIDDB2014&amp;lang=en</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/restsdmx/sdmx.ashx/GetData/GIDDB2014/ (SDMX)</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/SDMX-JSON/data/GIDDB2014/all/ (SDMX-JSON)</t>
+  </si>
+  <si>
+    <t>Gender, Institutions and Development (Edition 2012)</t>
+  </si>
+  <si>
+    <t>http://www.oecd-ilibrary.org/development/data/oecd-international-development-statistics/gender-institutions-and-development_data-00026-en</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/viewhtml.aspx?datasetcode=GIDDB2012&amp;lang=en</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/restsdmx/sdmx.ashx/GetData/GIDDB2012/ (SDMX)</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/SDMX-JSON/data/GIDDB2012/all/ (SDMX-JSON)</t>
+  </si>
+  <si>
+    <t>Gender, Institutions and Development Database 2009 (GID-DB)</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/viewhtml.aspx?datasetcode=GID2&amp;lang=en </t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/restsdmx/sdmx.ashx/GetData/GID2/ (SDMX)</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/SDMX-JSON/data/GID2/all/ (SDMX-JSON)</t>
+  </si>
+  <si>
+    <t>SIGI 2014</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/viewhtml.aspx?datasetcode=SIGI2014&amp;lang=en</t>
+  </si>
+  <si>
+    <t>Gender, Institutions adn Development DataBase 2014</t>
+  </si>
+  <si>
+    <t>Gender, Institutions adn Development DataBase 2012</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/restsdmx/sdmx.ashx/GetData/SIGI2014/ (SDMX)</t>
+  </si>
+  <si>
+    <t>http://stats.oecd.org/SDMX-JSON/data/SIGI2014/all/ (SDMX-JSON)</t>
+  </si>
+  <si>
+    <t>SIGI 2012</t>
+  </si>
+  <si>
+    <t>Download by hand</t>
+  </si>
+  <si>
+    <t>SIGI 2009</t>
+  </si>
+  <si>
+    <t>Gender, Institutions adn Development DataBase 2009</t>
+  </si>
+  <si>
+    <t>not available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -157,8 +233,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -171,6 +265,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -181,7 +287,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -191,8 +297,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -203,16 +313,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="9" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+  <cellStyles count="10">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,18 +659,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="12.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -810,4 +928,164 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="62.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="10" customFormat="1">
+      <c r="A1" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="8" customFormat="1">
+      <c r="A3" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="8" customFormat="1">
+      <c r="A7" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="10" customFormat="1">
+      <c r="A13" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="8" customFormat="1">
+      <c r="A15" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" s="8" customFormat="1">
+      <c r="A19" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="5" customFormat="1">
+      <c r="A20" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="10" customFormat="1">
+      <c r="A22" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="8" customFormat="1">
+      <c r="A23" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="8" customFormat="1">
+      <c r="A28" s="7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" s="5" customFormat="1">
+      <c r="A29" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3" display="http://stats.oecd.org/restsdmx/sdmx.ashx/GetData/GIDDB2014/"/>
+    <hyperlink ref="A6" r:id="rId4" display="http://stats.oecd.org/SDMX-JSON/data/GIDDB2014/all/"/>
+    <hyperlink ref="A14" r:id="rId5"/>
+    <hyperlink ref="A16" r:id="rId6"/>
+    <hyperlink ref="A17" r:id="rId7" display="http://stats.oecd.org/restsdmx/sdmx.ashx/GetData/GIDDB2014/"/>
+    <hyperlink ref="A18" r:id="rId8" display="http://stats.oecd.org/SDMX-JSON/data/GIDDB2014/all/"/>
+    <hyperlink ref="A24" r:id="rId9" display="http://stats.oecd.org/viewhtml.aspx?datasetcode=GID2&amp;lang=en"/>
+    <hyperlink ref="A25" r:id="rId10" display="http://stats.oecd.org/restsdmx/sdmx.ashx/GetData/GID2/"/>
+    <hyperlink ref="A26" r:id="rId11"/>
+    <hyperlink ref="A8" r:id="rId12"/>
+    <hyperlink ref="A9" r:id="rId13"/>
+    <hyperlink ref="A10" r:id="rId14"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated Land Matrix importer in order to be abe to process new LM XML data
</commit_message>
<xml_diff>
--- a/Simple_XLS_Importer/data/OECD-SIGI/SIGI_Recap.xlsx
+++ b/Simple_XLS_Importer/data/OECD-SIGI/SIGI_Recap.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\landbook-importers\Simple_XLS_Importer\data\OECD-SIGI\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-25640" yWindow="-440" windowWidth="25600" windowHeight="9520" tabRatio="500"/>
+    <workbookView xWindow="-25644" yWindow="-444" windowWidth="25596" windowHeight="9516" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="SIGI_recap" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="38">
   <si>
     <t>SIGI _ Recap</t>
   </si>
@@ -140,11 +145,29 @@
   <si>
     <t>NOTE: in green --&gt; Indicators just added</t>
   </si>
+  <si>
+    <t>Restricted access to productive and financial resources</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Not present. Generated it?</t>
+  </si>
+  <si>
+    <t>ok (removed Code in the title)</t>
+  </si>
+  <si>
+    <t>?. Not divided</t>
+  </si>
+  <si>
+    <t>Secure access to land assets - law + Secure access to land assets - practice?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -251,18 +274,26 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -588,25 +619,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="12.296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.296875" style="2" customWidth="1"/>
+    <col min="3" max="5" width="10.796875" style="2"/>
+    <col min="6" max="6" width="49.796875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>25</v>
       </c>
@@ -622,8 +655,11 @@
       <c r="E2" s="3">
         <v>2014</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="3">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -639,8 +675,11 @@
       <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -656,8 +695,11 @@
       <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -673,8 +715,11 @@
       <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -690,8 +735,11 @@
       <c r="E6" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -707,8 +755,11 @@
       <c r="E7" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -724,8 +775,11 @@
       <c r="E8" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -741,8 +795,11 @@
       <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -758,8 +815,11 @@
       <c r="E10" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -775,8 +835,11 @@
       <c r="E11" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -792,8 +855,11 @@
       <c r="E12" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -809,8 +875,11 @@
       <c r="E13" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -826,8 +895,11 @@
       <c r="E14" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -843,8 +915,11 @@
       <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="F15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>31</v>
       </c>
@@ -855,7 +930,7 @@
     <sortCondition ref="A3:A15"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>